<commit_message>
added teams and code for team colours
</commit_message>
<xml_diff>
--- a/hs_feb.xlsx
+++ b/hs_feb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2135339w_student_gla_ac_uk/Documents/Projects/hs/hs_feb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_9FF4AC7C9CB0901173FC1974DC7300627EEB5E2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAE38FFB-4B85-40D2-8050-28FB2BD2887A}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="11_9FF4AC7C9CB0901173FC1974DC7300627EEB5E2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29DA1A43-3A71-43C2-B96C-FBEB02BEA18F}"/>
   <bookViews>
     <workbookView xWindow="15825" yWindow="17190" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,21 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
   <si>
     <t>Zest</t>
-  </si>
-  <si>
-    <t>Simba</t>
   </si>
   <si>
     <t>Team</t>
   </si>
   <si>
     <t>Player</t>
-  </si>
-  <si>
-    <t>NickNack</t>
   </si>
   <si>
     <t>PP Huge</t>
@@ -65,9 +59,6 @@
     <t>Avion</t>
   </si>
   <si>
-    <t>Kal</t>
-  </si>
-  <si>
     <t>Time Machine</t>
   </si>
   <si>
@@ -76,12 +67,36 @@
   <si>
     <t>Jango</t>
   </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>YY</t>
+  </si>
+  <si>
+    <t>Sabbath</t>
+  </si>
+  <si>
+    <t>EZ</t>
+  </si>
+  <si>
+    <t>Nmbstr</t>
+  </si>
+  <si>
+    <t>Orion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +113,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,13 +140,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,18 +367,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1000"/>
+  <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.7109375" customWidth="1"/>
+    <col min="1" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" customWidth="1"/>
@@ -372,25 +394,26 @@
     <col min="18" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -400,424 +423,384 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
         <v>22.1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
         <v>22.2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="2"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>22.3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3">
+        <v>22.52</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>22.25</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="2"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>22.45</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3">
+        <v>22.71</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="2"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3">
+        <v>22.26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>22.46</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>22.71</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3">
+        <v>22.63</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="2"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="2"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="2"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="2"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="2"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="2"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="2"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="2"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="2"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="2"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -826,16 +809,16 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="2"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -844,14 +827,15 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="2"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -869,7 +853,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
@@ -888,7 +872,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
@@ -907,7 +891,7 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
     </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
@@ -926,7 +910,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
@@ -945,7 +929,7 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
@@ -964,7 +948,7 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
     </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -982,7 +966,7 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
     </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
@@ -1001,7 +985,7 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
     </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
@@ -1020,10 +1004,10 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
     </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1993,11 +1977,12 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N2:N28 H2:H28 K2:K28 Q2:Q28 E2:E28" xr:uid="{906058B7-BD67-498C-B2B3-7B679D620D42}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N20:N28 F2:F19 E20:E28 R2:R19 Q20:Q28 L2:L19 K20:K28 I2:I19 H20:H28 O2:O19" xr:uid="{906058B7-BD67-498C-B2B3-7B679D620D42}">
       <formula1>"Factory,Beach,Atlantic Road,Rocky Mountain,River Peak,Oasis,Jungle,Mt. Hairpin,New Hong Kong"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M2:M28 J2:J28 G2:G28 P2:P28 D2:D28" xr:uid="{BE70E1DA-6A1E-4496-B4E2-E3E1E11BC546}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M20:M28 E2:E19 D20:D28 Q2:Q19 P20:P28 H17:H19 G20:G28 K2:K19 J20:J28 N2:N19" xr:uid="{BE70E1DA-6A1E-4496-B4E2-E3E1E11BC546}">
       <formula1>"Time Machine,Fury,Ghost,Satin,Coupe,Leap,Maverick,Hornet,Bandit,Wild West,Firearrow,Nighttown,Taxi,Atomic,Predator,Bison,Monster Truck,Hopper,Hammer,Fortress,Ronin,Kobra,Comet,Mamba,Wingman,Koi,Horizon,Electron,Cyber Truck,Flower,The Krystal Ship,Mini"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added in day 1 data and adjusted figure
</commit_message>
<xml_diff>
--- a/hs_feb.xlsx
+++ b/hs_feb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2135339w_student_gla_ac_uk/Documents/Projects/hs/hs_feb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="11_9FF4AC7C9CB0901173FC1974DC7300627EEB5E2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29DA1A43-3A71-43C2-B96C-FBEB02BEA18F}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_77BC072D2A3A8E8771E1F836A3C0E5F2BF667978" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1DA4947-BC41-4725-97F4-6D904A693B4A}"/>
   <bookViews>
-    <workbookView xWindow="15825" yWindow="17190" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,81 +28,213 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="dJ4Rh94lPtlVPTM6a+k/LVkmxz6tdKOBxjoHCTfALj4="/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="64">
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Time_1</t>
+  </si>
+  <si>
+    <t>Car_1</t>
+  </si>
+  <si>
+    <t>Track_1</t>
+  </si>
+  <si>
+    <t>Time_2</t>
+  </si>
+  <si>
+    <t>Car_2</t>
+  </si>
+  <si>
+    <t>Track_2</t>
+  </si>
+  <si>
+    <t>Time_3</t>
+  </si>
+  <si>
+    <t>Car_3</t>
+  </si>
+  <si>
+    <t>Track_3</t>
+  </si>
+  <si>
+    <t>Time_4</t>
+  </si>
+  <si>
+    <t>Car_4</t>
+  </si>
+  <si>
+    <t>Track_4</t>
+  </si>
+  <si>
+    <t>Time_5</t>
+  </si>
+  <si>
+    <t>Car_5</t>
+  </si>
+  <si>
+    <t>Track_5</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>Jango</t>
+  </si>
+  <si>
+    <t>Time Machine</t>
+  </si>
+  <si>
+    <t>Atlantic Road</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>PP Huge</t>
+  </si>
   <si>
     <t>Zest</t>
   </si>
   <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>Player</t>
-  </si>
-  <si>
-    <t>PP Huge</t>
-  </si>
-  <si>
-    <t>Time_1</t>
-  </si>
-  <si>
-    <t>Car_1</t>
-  </si>
-  <si>
-    <t>Track_1</t>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>YY</t>
+  </si>
+  <si>
+    <t>Tattoo</t>
+  </si>
+  <si>
+    <t>EZ</t>
+  </si>
+  <si>
+    <t>Ridge</t>
+  </si>
+  <si>
+    <t>Fawn</t>
+  </si>
+  <si>
+    <t>Muffin</t>
+  </si>
+  <si>
+    <t>Chungus</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Kalaginho</t>
+  </si>
+  <si>
+    <t>Motski</t>
+  </si>
+  <si>
+    <t>KenDan</t>
+  </si>
+  <si>
+    <t>Stay Behind</t>
+  </si>
+  <si>
+    <t>NickNack</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Voh</t>
+  </si>
+  <si>
+    <t>Beagle</t>
+  </si>
+  <si>
+    <t>Orion</t>
+  </si>
+  <si>
+    <t>Kal</t>
+  </si>
+  <si>
+    <t>Littorio</t>
+  </si>
+  <si>
+    <t>Ryuzu</t>
+  </si>
+  <si>
+    <t>Kaizen</t>
   </si>
   <si>
     <t>Avion</t>
   </si>
   <si>
-    <t>Time Machine</t>
-  </si>
-  <si>
-    <t>Atlantic Road</t>
-  </si>
-  <si>
-    <t>Jango</t>
+    <t>Bean</t>
+  </si>
+  <si>
+    <t>Balla</t>
+  </si>
+  <si>
+    <t>Snowman</t>
+  </si>
+  <si>
+    <t>Nmbstr</t>
+  </si>
+  <si>
+    <t>Larz</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>Chooch</t>
+  </si>
+  <si>
+    <t>Calmeh</t>
+  </si>
+  <si>
+    <t>Kenny Powers</t>
+  </si>
+  <si>
+    <t>Sabbath</t>
+  </si>
+  <si>
+    <t>Aspect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luk </t>
+  </si>
+  <si>
+    <t>Joes</t>
+  </si>
+  <si>
+    <t>JonReremy</t>
+  </si>
+  <si>
+    <t>Mt. Hairpin</t>
   </si>
   <si>
     <t>Colour</t>
   </si>
   <si>
-    <t>TD</t>
-  </si>
-  <si>
-    <t>NN</t>
-  </si>
-  <si>
-    <t>YY</t>
-  </si>
-  <si>
-    <t>Sabbath</t>
-  </si>
-  <si>
-    <t>EZ</t>
-  </si>
-  <si>
-    <t>Nmbstr</t>
-  </si>
-  <si>
-    <t>Orion</t>
+    <t>Koi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,7 +247,8 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -140,14 +273,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,10 +295,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,20 +498,21 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F37" sqref="F37:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
     <col min="13" max="13" width="20.140625" customWidth="1"/>
@@ -391,639 +520,1281 @@
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
     <col min="16" max="16" width="19.28515625" customWidth="1"/>
     <col min="17" max="17" width="17.42578125" customWidth="1"/>
-    <col min="18" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
-        <v>22.1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D2" s="1">
+        <v>22.32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3">
-        <v>22.2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>22.36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3">
-        <v>22.52</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="D4" s="1">
+        <v>22.4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D5" s="3">
-        <v>22.25</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+        <v>22.43</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3">
+        <v>22.45</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1">
+        <v>22.53</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3">
-        <v>22.71</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3">
-        <v>22.26</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1">
+        <v>22.59</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3">
         <v>22.63</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1">
+        <v>22.631</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1">
+        <v>22.632000000000001</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1">
+        <v>22.67</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3">
+        <v>22.69</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1">
+        <v>22.690999999999999</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1">
+        <v>22.74</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1">
+        <v>22.75</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1">
+        <v>22.76</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1">
+        <v>22.760999999999999</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="1">
+        <v>22.78</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-    </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-    </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-    </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-    </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1">
+        <v>22.8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="3">
+        <v>22.86</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="1">
+        <v>22.87</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="1">
+        <v>22.88</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="1">
+        <v>22.9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="3">
+        <v>22.901</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="3">
+        <v>22.92</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+    </row>
+    <row r="27" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="1">
+        <v>22.920999999999999</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+    </row>
+    <row r="28" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="1">
+        <v>22.98</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+    </row>
+    <row r="29" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="1">
+        <v>23.03</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+    </row>
+    <row r="30" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="1">
+        <v>23.07</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+    </row>
+    <row r="31" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="1">
+        <v>23.12</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+    </row>
+    <row r="32" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="1">
+        <v>23.34</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+    </row>
+    <row r="33" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="1">
+        <v>23.42</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="3">
+        <v>23.47</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="3">
+        <v>23.78</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+    </row>
+    <row r="36" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="1">
+        <f>24.83/1.0185/1.0185</f>
+        <v>23.936169571807184</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+    </row>
+    <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1977,13 +2748,12 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N20:N28 F2:F19 E20:E28 R2:R19 Q20:Q28 L2:L19 K20:K28 I2:I19 H20:H28 O2:O19" xr:uid="{906058B7-BD67-498C-B2B3-7B679D620D42}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E38 Q2:Q37 K2:K37 N2:N37 H2:H38" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"Time Machine,Fury,Ghost,Satin,Coupe,Leap,Maverick,Hornet,Bandit,Wild West,Firearrow,Nighttown,Taxi,Atomic,Predator,Bison,Monster Truck,Hopper,Hammer,Fortress,Ronin,Kobra,Comet,Mamba,Wingman,Koi,Horizon,Electron,Cyber Truck,Flower,The Krystal Ship,Mini"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F38 R2:R37 L2:L37 O2:O37 I2:I38" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Factory,Beach,Atlantic Road,Rocky Mountain,River Peak,Oasis,Jungle,Mt. Hairpin,New Hong Kong"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M20:M28 E2:E19 D20:D28 Q2:Q19 P20:P28 H17:H19 G20:G28 K2:K19 J20:J28 N2:N19" xr:uid="{BE70E1DA-6A1E-4496-B4E2-E3E1E11BC546}">
-      <formula1>"Time Machine,Fury,Ghost,Satin,Coupe,Leap,Maverick,Hornet,Bandit,Wild West,Firearrow,Nighttown,Taxi,Atomic,Predator,Bison,Monster Truck,Hopper,Hammer,Fortress,Ronin,Kobra,Comet,Mamba,Wingman,Koi,Horizon,Electron,Cyber Truck,Flower,The Krystal Ship,Mini"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
changed dw score NAs to 0
</commit_message>
<xml_diff>
--- a/hs_feb.xlsx
+++ b/hs_feb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2135339w_student_gla_ac_uk/Documents/Projects/hs/hs_feb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_77BC072D2A3A8E8771E1F836A3C0E5F2BF667978" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1DA4947-BC41-4725-97F4-6D904A693B4A}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_77BC072D2A3A8E8771E1F836A3C0E5F2BF667978" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A008D461-4108-487A-819B-B8E25A915CA4}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="50">
   <si>
     <t>Team</t>
   </si>
@@ -53,42 +53,6 @@
     <t>Track_1</t>
   </si>
   <si>
-    <t>Time_2</t>
-  </si>
-  <si>
-    <t>Car_2</t>
-  </si>
-  <si>
-    <t>Track_2</t>
-  </si>
-  <si>
-    <t>Time_3</t>
-  </si>
-  <si>
-    <t>Car_3</t>
-  </si>
-  <si>
-    <t>Track_3</t>
-  </si>
-  <si>
-    <t>Time_4</t>
-  </si>
-  <si>
-    <t>Car_4</t>
-  </si>
-  <si>
-    <t>Track_4</t>
-  </si>
-  <si>
-    <t>Time_5</t>
-  </si>
-  <si>
-    <t>Car_5</t>
-  </si>
-  <si>
-    <t>Track_5</t>
-  </si>
-  <si>
     <t>TD</t>
   </si>
   <si>
@@ -221,13 +185,7 @@
     <t>JonReremy</t>
   </si>
   <si>
-    <t>Mt. Hairpin</t>
-  </si>
-  <si>
     <t>Colour</t>
-  </si>
-  <si>
-    <t>Koi</t>
   </si>
 </sst>
 </file>
@@ -295,6 +253,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,7 +460,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:F38"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -524,7 +486,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -541,66 +503,38 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1">
         <v>22.32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -613,27 +547,23 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>22.36</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -646,27 +576,23 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>22.4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -679,27 +605,23 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3">
         <v>22.43</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -712,27 +634,23 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
         <v>22.45</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -745,27 +663,23 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1">
         <v>22.53</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -778,27 +692,23 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D8" s="1">
         <v>22.59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -811,27 +721,23 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3">
         <v>22.63</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -844,27 +750,23 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1">
         <v>22.631</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -877,27 +779,23 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1">
         <v>22.632000000000001</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -910,27 +808,23 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1">
         <v>22.67</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -943,27 +837,23 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3">
         <v>22.69</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -976,27 +866,23 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1">
         <v>22.690999999999999</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1009,27 +895,23 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1">
         <v>22.74</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1042,27 +924,23 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1">
         <v>22.75</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1075,27 +953,23 @@
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1">
         <v>22.76</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1108,27 +982,23 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1">
         <v>22.760999999999999</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1141,27 +1011,23 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D19" s="1">
         <v>22.78</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1174,27 +1040,23 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1">
         <v>22.8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1207,27 +1069,23 @@
     </row>
     <row r="21" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D21" s="3">
         <v>22.86</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1240,27 +1098,23 @@
     </row>
     <row r="22" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D22" s="1">
         <v>22.87</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1273,27 +1127,23 @@
     </row>
     <row r="23" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1">
         <v>22.88</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1306,27 +1156,23 @@
     </row>
     <row r="24" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D24" s="1">
         <v>22.9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1339,27 +1185,23 @@
     </row>
     <row r="25" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D25" s="3">
         <v>22.901</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1372,27 +1214,23 @@
     </row>
     <row r="26" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D26" s="3">
         <v>22.92</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1405,27 +1243,23 @@
     </row>
     <row r="27" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D27" s="1">
         <v>22.920999999999999</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1438,27 +1272,23 @@
     </row>
     <row r="28" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D28" s="1">
         <v>22.98</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1471,27 +1301,23 @@
     </row>
     <row r="29" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D29" s="1">
         <v>23.03</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1504,27 +1330,23 @@
     </row>
     <row r="30" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D30" s="1">
         <v>23.07</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1537,27 +1359,23 @@
     </row>
     <row r="31" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D31" s="1">
         <v>23.12</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1570,27 +1388,23 @@
     </row>
     <row r="32" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D32" s="1">
         <v>23.34</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1603,27 +1417,23 @@
     </row>
     <row r="33" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D33" s="1">
         <v>23.42</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1636,27 +1446,23 @@
     </row>
     <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D34" s="3">
         <v>23.47</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1669,27 +1475,23 @@
     </row>
     <row r="35" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D35" s="3">
         <v>23.78</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1702,28 +1504,24 @@
     </row>
     <row r="36" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D36" s="1">
         <f>24.83/1.0185/1.0185</f>
         <v>23.936169571807184</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1736,25 +1534,21 @@
     </row>
     <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1767,23 +1561,19 @@
     </row>
     <row r="38" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
     </row>
     <row r="39" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added day 2 results and fixed bug in final_df()
</commit_message>
<xml_diff>
--- a/hs_feb.xlsx
+++ b/hs_feb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2135339w_student_gla_ac_uk/Documents/Projects/hs/hs_feb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_77BC072D2A3A8E8771E1F836A3C0E5F2BF667978" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5909335C-E8A6-4D3A-9D54-CFC9197E0F10}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_77BC072D2A3A8E8771E1F836A3C0E5F2BF667978" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FBFDEA7-793F-4D60-9E29-687C66F72600}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="54">
   <si>
     <t>Team</t>
   </si>
@@ -183,17 +183,39 @@
   </si>
   <si>
     <t>Colour</t>
+  </si>
+  <si>
+    <t>Time_2</t>
+  </si>
+  <si>
+    <t>Car_2</t>
+  </si>
+  <si>
+    <t>Track_2</t>
+  </si>
+  <si>
+    <t>Koi</t>
+  </si>
+  <si>
+    <t>Mt. Hairpin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -207,6 +229,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,7 +244,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -224,17 +252,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -481,7 +531,7 @@
     <col min="17" max="17" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -500,9 +550,15 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="G1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -513,7 +569,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -529,9 +585,15 @@
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="G2" s="4">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -542,7 +604,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
@@ -558,9 +620,15 @@
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="G3" s="4">
+        <v>32.64</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -571,7 +639,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
@@ -587,9 +655,15 @@
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="G4" s="4">
+        <v>32.82</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -600,7 +674,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -616,9 +690,15 @@
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="G5" s="4">
+        <v>33.18</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -629,7 +709,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -645,9 +725,15 @@
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="G6" s="4">
+        <v>33.020000000000003</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -658,7 +744,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -674,9 +760,15 @@
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="G7" s="4">
+        <v>32.840000000000003</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -687,7 +779,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -703,9 +795,15 @@
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="G8" s="4">
+        <v>33.99</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -716,7 +814,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -732,9 +830,15 @@
       <c r="F9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="G9" s="4">
+        <v>33.191000000000003</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -745,7 +849,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -761,9 +865,15 @@
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="G10" s="4">
+        <v>32.92</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -774,7 +884,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -790,9 +900,15 @@
       <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="G11" s="4">
+        <v>33.270000000000003</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -803,7 +919,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
@@ -819,9 +935,15 @@
       <c r="F12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="G12" s="4">
+        <v>33.54</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -832,7 +954,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -848,9 +970,15 @@
       <c r="F13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="4">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -861,7 +989,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
@@ -877,9 +1005,15 @@
       <c r="F14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="G14" s="4">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -890,7 +1024,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
@@ -906,9 +1040,15 @@
       <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="G15" s="4">
+        <v>34.17</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -919,7 +1059,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
@@ -935,9 +1075,15 @@
       <c r="F16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="G16" s="4">
+        <v>33.19</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -948,7 +1094,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
@@ -964,9 +1110,15 @@
       <c r="F17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="G17" s="4">
+        <v>33.93</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -977,7 +1129,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
@@ -993,9 +1145,15 @@
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="4">
+        <v>33.450000000000003</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1006,7 +1164,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1022,9 +1180,15 @@
       <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="G19" s="4">
+        <v>33.58</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1035,7 +1199,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>5</v>
       </c>
@@ -1051,9 +1215,15 @@
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="G20" s="4">
+        <v>33.43</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1064,7 +1234,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1080,9 +1250,15 @@
       <c r="F21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="G21" s="4">
+        <v>32.99</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1093,7 +1269,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1109,9 +1285,15 @@
       <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="G22" s="4">
+        <v>34.020000000000003</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1122,7 +1304,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1138,9 +1320,15 @@
       <c r="F23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="G23" s="4">
+        <v>33.11</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1151,7 +1339,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>5</v>
       </c>
@@ -1167,9 +1355,15 @@
       <c r="F24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="G24" s="4">
+        <v>33.450000000000003</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1180,7 +1374,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
@@ -1196,9 +1390,15 @@
       <c r="F25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="G25" s="4">
+        <v>33.89</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1209,7 +1409,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
@@ -1225,9 +1425,15 @@
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="G26" s="4">
+        <v>34.57</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1238,7 +1444,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
@@ -1254,9 +1460,15 @@
       <c r="F27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="G27" s="4">
+        <v>33.78</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1267,7 +1479,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
@@ -1283,9 +1495,15 @@
       <c r="F28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="G28" s="4">
+        <v>34.14</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1296,7 +1514,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1312,9 +1530,15 @@
       <c r="F29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="G29" s="4">
+        <v>33.79</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1325,7 +1549,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>9</v>
       </c>
@@ -1341,9 +1565,15 @@
       <c r="F30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="G30" s="4">
+        <v>34.659999999999997</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1354,7 +1584,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
@@ -1370,9 +1600,15 @@
       <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="G31" s="4">
+        <v>33.81</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1383,7 +1619,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>5</v>
       </c>
@@ -1399,9 +1635,15 @@
       <c r="F32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="G32" s="4">
+        <v>34.46</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1412,7 +1654,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1428,9 +1670,15 @@
       <c r="F33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="G33" s="4">
+        <v>35.22</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1441,7 +1689,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
@@ -1457,9 +1705,15 @@
       <c r="F34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="G34" s="4">
+        <v>33.71</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1470,7 +1724,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>26</v>
       </c>
@@ -1487,9 +1741,13 @@
       <c r="F35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1500,7 +1758,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
@@ -1514,9 +1772,15 @@
       <c r="F36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="G36" s="4">
+        <v>35.68</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1527,7 +1791,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>5</v>
       </c>
@@ -1540,9 +1804,15 @@
       <c r="F37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="G37" s="4">
+        <v>32.729999999999997</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -2521,10 +2791,10 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q2:Q37 K2:K37 N2:N37 H2:H38 E2:E37" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q2:Q37 K2:K37 N2:N37 E2:E37 H2:H38" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Time Machine,Fury,Ghost,Satin,Coupe,Leap,Maverick,Hornet,Bandit,Wild West,Firearrow,Nighttown,Taxi,Atomic,Predator,Bison,Monster Truck,Hopper,Hammer,Fortress,Ronin,Kobra,Comet,Mamba,Wingman,Koi,Horizon,Electron,Cyber Truck,Flower,The Krystal Ship,Mini"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="R2:R37 L2:L37 O2:O37 I2:I38 F2:F37" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="R2:R37 L2:L37 O2:O37 F2:F37 I2:I38" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Factory,Beach,Atlantic Road,Rocky Mountain,River Peak,Oasis,Jungle,Mt. Hairpin,New Hong Kong"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>